<commit_message>
Changed household_new survey to take advantage of more linked_table functionality
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
   <si>
     <t>comments</t>
   </si>
@@ -120,9 +120,6 @@
     <t>household_new</t>
   </si>
   <si>
-    <t>household_member</t>
-  </si>
-  <si>
     <t>imnci_test</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/household/forms/household_new/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/household_member/forms/household_member/',null)</t>
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/imnci/forms/imnci_test/',null)</t>
@@ -252,8 +246,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -312,7 +312,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -334,6 +334,9 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -355,6 +358,9 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -691,10 +697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -710,10 +716,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -725,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -752,7 +758,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" customHeight="1">
@@ -779,7 +785,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" customHeight="1">
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1">
@@ -791,45 +797,45 @@
     <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
         <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
         <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.5" customHeight="1">
@@ -841,20 +847,20 @@
     <row r="15" spans="1:9" ht="66" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
         <v>42</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1">
@@ -865,20 +871,20 @@
     <row r="18" spans="1:7" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
         <v>42</v>
-      </c>
-      <c r="G18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1">
@@ -889,20 +895,20 @@
     <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
         <v>42</v>
-      </c>
-      <c r="G21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1">
@@ -913,20 +919,20 @@
     <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="s">
         <v>42</v>
-      </c>
-      <c r="G24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1">
@@ -937,20 +943,20 @@
     <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" t="s">
         <v>42</v>
-      </c>
-      <c r="G27" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1">
@@ -961,20 +967,20 @@
     <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" t="s">
         <v>42</v>
-      </c>
-      <c r="G30" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1">
@@ -985,20 +991,20 @@
     <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" t="s">
         <v>42</v>
-      </c>
-      <c r="G33" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1">
@@ -1009,25 +1015,25 @@
     <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" t="s">
         <v>42</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1">
@@ -1036,41 +1042,17 @@
         <v>57</v>
       </c>
       <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G39" t="s">
         <v>42</v>
-      </c>
-      <c r="G39" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="17" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1">
@@ -1120,7 +1102,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
@@ -1220,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1260,10 +1242,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1359,25 +1341,15 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Include grid screen functionality
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>comments</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>showContents</t>
+  </si>
+  <si>
+    <t>gridScreen</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/gridScreen/forms/gridScreen/',null)</t>
   </si>
 </sst>
 </file>
@@ -246,8 +252,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -312,7 +322,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -337,6 +347,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -361,6 +373,8 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,10 +711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1052,6 +1066,30 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="66" customHeight="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17" customHeight="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1202,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1347,6 +1385,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add child and adult coverage immunization forms
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
   <si>
     <t>comments</t>
   </si>
@@ -205,6 +205,24 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/gridScreen/forms/gridScreen/',null)</t>
+  </si>
+  <si>
+    <t>adult_coverage</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/adult_coverage/forms/adult_coverage/',null)</t>
+  </si>
+  <si>
+    <t>child_coverage</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/child_coverage/forms/child_coverage/',null)</t>
+  </si>
+  <si>
+    <t>Child Coverage Immunizations</t>
+  </si>
+  <si>
+    <t>Adult Coverage Immunizations</t>
   </si>
 </sst>
 </file>
@@ -252,8 +270,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,7 +346,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -349,6 +373,9 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -375,6 +402,9 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -711,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1090,6 +1120,54 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="66" customHeight="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17" customHeight="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="66" customHeight="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" customHeight="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1240,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1396,6 +1474,28 @@
         <v>59</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Intermediate check-in of graph prompt types
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="19200" yWindow="2040" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
   <si>
     <t>comments</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>Adult Coverage Immunizations</t>
+  </si>
+  <si>
+    <t>graphExample</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/graphExample/forms/graphExample/',null)</t>
+  </si>
+  <si>
+    <t>Graph Examples</t>
   </si>
 </sst>
 </file>
@@ -270,8 +279,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,7 +359,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -376,6 +389,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +420,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,10 +758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1164,10 +1181,34 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17" customHeight="1">
+    <row r="49" spans="1:7" ht="17" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="66" customHeight="1">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" t="s">
+        <v>41</v>
+      </c>
+      <c r="G51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17" customHeight="1">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1318,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1496,6 +1537,17 @@
         <v>66</v>
       </c>
     </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
New forms for the BMGF demo
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="2040" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="10560" yWindow="1920" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
   <si>
     <t>comments</t>
   </si>
@@ -232,6 +232,24 @@
   </si>
   <si>
     <t>Graph Examples</t>
+  </si>
+  <si>
+    <t>visit</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/visit/forms/visit/',null)</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/plot/forms/plot/',null)</t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>Plot</t>
   </si>
 </sst>
 </file>
@@ -279,8 +297,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -359,7 +383,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -391,6 +415,9 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -422,6 +449,9 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1209,6 +1239,54 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="66" customHeight="1">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" t="s">
+        <v>41</v>
+      </c>
+      <c r="G54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17" customHeight="1">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="66" customHeight="1">
+      <c r="A57" s="3"/>
+      <c r="B57" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17" customHeight="1">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1359,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1548,6 +1626,28 @@
         <v>69</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
new branch for the newer version of study mPneumonia Path is using
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1920" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
   <si>
     <t>comments</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Plot</t>
+  </si>
+  <si>
+    <t>mPneumonia</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/mPneumonia/forms/mPneumonia/',null)</t>
   </si>
 </sst>
 </file>
@@ -297,8 +303,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +391,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +426,7 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +461,7 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -880,40 +890,33 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" customHeight="1">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="59" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -931,14 +934,14 @@
     </row>
     <row r="14" spans="1:9" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="59" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -955,14 +958,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -980,13 +984,13 @@
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1004,13 +1008,13 @@
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1028,13 +1032,13 @@
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1052,13 +1056,13 @@
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1076,13 +1080,13 @@
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1100,13 +1104,13 @@
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1124,13 +1128,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1148,13 +1152,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1172,13 +1176,13 @@
     </row>
     <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1196,13 +1200,13 @@
     </row>
     <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -1220,13 +1224,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
         <v>41</v>
@@ -1244,13 +1248,13 @@
     </row>
     <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
         <v>41</v>
@@ -1268,13 +1272,13 @@
     </row>
     <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
         <v>41</v>
@@ -1287,6 +1291,30 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="66" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" customHeight="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1437,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1462,14 +1490,14 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1477,10 +1505,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1488,21 +1516,21 @@
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1510,10 +1538,10 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1521,10 +1549,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1532,10 +1560,10 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1543,10 +1571,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1554,10 +1582,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1565,10 +1593,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1576,10 +1604,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1587,10 +1615,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1598,10 +1626,10 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1609,10 +1637,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1620,10 +1648,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1631,10 +1659,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1642,9 +1670,20 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Old Version of Survey used by mPneumonia Path group
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1920" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
   <si>
     <t>comments</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Plot</t>
+  </si>
+  <si>
+    <t>mPneumonia</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/mPneumonia/forms/mPneumonia/',null)</t>
   </si>
 </sst>
 </file>
@@ -297,8 +303,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +391,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +426,7 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +461,7 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -881,14 +891,14 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
@@ -904,16 +914,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1">
+    <row r="11" spans="1:9" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -931,14 +941,14 @@
     </row>
     <row r="14" spans="1:9" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="59" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -955,14 +965,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -980,13 +991,13 @@
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1004,13 +1015,13 @@
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1028,13 +1039,13 @@
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1052,13 +1063,13 @@
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1076,13 +1087,13 @@
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1100,13 +1111,13 @@
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1124,13 +1135,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1148,13 +1159,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1172,13 +1183,13 @@
     </row>
     <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1196,13 +1207,13 @@
     </row>
     <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -1220,13 +1231,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
         <v>41</v>
@@ -1244,13 +1255,13 @@
     </row>
     <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
         <v>41</v>
@@ -1268,13 +1279,13 @@
     </row>
     <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
         <v>41</v>
@@ -1287,6 +1298,30 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="66" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" customHeight="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1437,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1462,14 +1497,14 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1477,10 +1512,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1488,21 +1523,21 @@
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1510,10 +1545,10 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1521,10 +1556,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1532,10 +1567,10 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1543,10 +1578,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1554,10 +1589,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1565,10 +1600,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1576,10 +1611,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1587,10 +1622,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1598,10 +1633,10 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1609,10 +1644,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1620,10 +1655,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1631,10 +1666,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1642,9 +1677,20 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add geotagger to the framework so that it can be used in demos
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
   <si>
     <t>comments</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Plot</t>
+  </si>
+  <si>
+    <t>geotagger</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/geotagger/forms/geotagger/',null)</t>
+  </si>
+  <si>
+    <t>Geotagger</t>
   </si>
 </sst>
 </file>
@@ -297,8 +306,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +400,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +435,10 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +473,10 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -881,14 +906,14 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
@@ -904,16 +929,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1">
+    <row r="11" spans="1:9" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -931,14 +956,14 @@
     </row>
     <row r="14" spans="1:9" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="59" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -955,14 +980,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -980,13 +1006,13 @@
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1004,13 +1030,13 @@
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1028,13 +1054,13 @@
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1052,13 +1078,13 @@
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1076,13 +1102,13 @@
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1100,13 +1126,13 @@
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1124,13 +1150,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1148,13 +1174,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1172,13 +1198,13 @@
     </row>
     <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1196,13 +1222,13 @@
     </row>
     <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -1220,13 +1246,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
         <v>41</v>
@@ -1244,13 +1270,13 @@
     </row>
     <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
         <v>41</v>
@@ -1268,13 +1294,13 @@
     </row>
     <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
         <v>41</v>
@@ -1287,6 +1313,30 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="66" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" customHeight="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1437,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1465,11 +1515,11 @@
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1477,10 +1527,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1488,21 +1538,21 @@
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1510,10 +1560,10 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1521,10 +1571,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1532,10 +1582,10 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1543,10 +1593,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1554,10 +1604,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1565,10 +1615,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1576,10 +1626,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1587,10 +1637,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1598,10 +1648,10 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1609,10 +1659,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1620,10 +1670,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1631,10 +1681,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1642,9 +1692,20 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct delete statement - SQLite doesn't like linked queries on deletes.
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1920" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="10560" yWindow="1920" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="84">
   <si>
     <t>comments</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/geoweather/forms/geoweather/',null)</t>
+  </si>
+  <si>
+    <t>agriculture</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/agriculture/forms/agriculture/',null)</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
   </si>
 </sst>
 </file>
@@ -819,10 +828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,14 +921,14 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
@@ -937,14 +946,14 @@
     </row>
     <row r="11" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -960,16 +969,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -987,14 +996,14 @@
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -1011,14 +1020,15 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1036,13 +1046,13 @@
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1060,13 +1070,13 @@
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1084,13 +1094,13 @@
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1108,13 +1118,13 @@
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1132,13 +1142,13 @@
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1156,13 +1166,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1180,13 +1190,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1204,13 +1214,13 @@
     </row>
     <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1228,13 +1238,13 @@
     </row>
     <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -1252,13 +1262,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
         <v>41</v>
@@ -1276,13 +1286,13 @@
     </row>
     <row r="53" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
         <v>41</v>
@@ -1300,13 +1310,13 @@
     </row>
     <row r="56" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E57" t="s">
         <v>41</v>
@@ -1324,13 +1334,13 @@
     </row>
     <row r="59" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E60" t="s">
         <v>41</v>
@@ -1348,13 +1358,13 @@
     </row>
     <row r="62" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E63" t="s">
         <v>41</v>
@@ -1367,6 +1377,30 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1517,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1744,9 +1778,20 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add ability to get data and send in sms.
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1920" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>comments</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>Agriculture</t>
+  </si>
+  <si>
+    <t>send_sms</t>
+  </si>
+  <si>
+    <t>Send SMS</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/send_sms/forms/send_sms/',null)</t>
   </si>
 </sst>
 </file>
@@ -321,8 +330,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -415,7 +426,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -454,6 +465,7 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -492,6 +504,7 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,13 +810,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,7 +824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -828,24 +841,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="101.1796875" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -872,7 +885,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17" customHeight="1">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -881,7 +894,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -892,13 +905,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17" customHeight="1">
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="41" customHeight="1">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -909,23 +922,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17" customHeight="1">
       <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17" customHeight="1">
       <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>82</v>
@@ -937,20 +950,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>77</v>
@@ -962,20 +975,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="59" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>46</v>
@@ -987,20 +1000,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="59" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>47</v>
@@ -1012,20 +1025,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="17" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>48</v>
@@ -1037,19 +1050,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="17" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>49</v>
@@ -1061,19 +1074,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>50</v>
@@ -1085,19 +1098,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>51</v>
@@ -1109,19 +1122,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>52</v>
@@ -1133,19 +1146,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="17" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>53</v>
@@ -1157,19 +1170,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="17" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>54</v>
@@ -1181,19 +1194,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="17" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>55</v>
@@ -1205,19 +1218,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="17" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
         <v>57</v>
@@ -1229,19 +1242,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="17" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
         <v>60</v>
@@ -1253,19 +1266,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="17" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>62</v>
@@ -1277,19 +1290,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="17" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
         <v>64</v>
@@ -1301,19 +1314,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="17" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
         <v>68</v>
@@ -1325,19 +1338,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="17" customHeight="1">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="66" customHeight="1">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
         <v>71</v>
@@ -1349,19 +1362,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="17" customHeight="1">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="17.5" customHeight="1">
       <c r="A62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="66" customHeight="1">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
         <v>73</v>
@@ -1373,19 +1386,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="17" customHeight="1">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="17.5" customHeight="1">
       <c r="A65" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="66" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
         <v>80</v>
@@ -1397,10 +1410,34 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="17" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="66" customHeight="1">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17" customHeight="1">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1423,13 +1460,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1483,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1458,7 +1495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1483,60 +1520,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1551,20 +1588,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1575,7 +1612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1586,7 +1623,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1597,7 +1634,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1608,7 +1645,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1656,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1630,7 +1667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1641,7 +1678,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +1689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1663,7 +1700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1674,7 +1711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1685,7 +1722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1696,7 +1733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1707,7 +1744,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1718,7 +1755,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1729,7 +1766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1740,7 +1777,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1751,7 +1788,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -1762,7 +1799,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1773,7 +1810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1784,7 +1821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -1793,6 +1830,17 @@
       </c>
       <c r="C21" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediate check-in of scan forms
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
   <si>
     <t>comments</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/send_sms/forms/send_sms/',null)</t>
+  </si>
+  <si>
+    <t>scan</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/scan_example/forms/scan_example/',null)</t>
+  </si>
+  <si>
+    <t>Scan</t>
   </si>
 </sst>
 </file>
@@ -330,8 +339,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,7 +439,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +479,8 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -505,6 +520,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -841,10 +858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1438,6 +1455,30 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="66" customHeight="1">
+      <c r="A72" s="3"/>
+      <c r="B72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" t="s">
+        <v>41</v>
+      </c>
+      <c r="G72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17" customHeight="1">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1588,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1843,6 +1884,17 @@
         <v>85</v>
       </c>
     </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Fix TOC in Survey for media, fix push tasks to not include framework, change framework.xlsx to not include scan
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>comments</t>
   </si>
@@ -283,15 +283,6 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/send_sms/forms/send_sms/',null)</t>
-  </si>
-  <si>
-    <t>scan</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/scan_example/forms/scan_example/',null)</t>
-  </si>
-  <si>
-    <t>Scan</t>
   </si>
 </sst>
 </file>
@@ -860,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1458,29 +1449,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A71" t="s">
-        <v>87</v>
-      </c>
-    </row>
+    <row r="71" spans="1:7" ht="17.5" customHeight="1"/>
     <row r="72" spans="1:7" ht="66" customHeight="1">
       <c r="A72" s="3"/>
-      <c r="B72" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E72" t="s">
-        <v>41</v>
-      </c>
-      <c r="G72" t="s">
-        <v>42</v>
-      </c>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:7" ht="17" customHeight="1">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
-      <c r="C73" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1884,17 +1860,6 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>